<commit_message>
setting up scrape, added columns to Teachers table, updated rake tasks and teacher import/truncate methods
</commit_message>
<xml_diff>
--- a/db/teachers.xlsx
+++ b/db/teachers.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="59">
   <si>
     <t>Adam Schwamb</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Dan Shure</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Stephanie Wirzburger</t>
   </si>
   <si>
@@ -186,16 +183,45 @@
   </si>
   <si>
     <t>Joe Davis</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Acme Piano</t>
+  </si>
+  <si>
+    <t>joe@acme.com</t>
+  </si>
+  <si>
+    <t>www.smithpiano.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,13 +244,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -500,290 +529,469 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>10</v>
       </c>
-      <c r="C19" t="s">
-        <v>51</v>
-      </c>
       <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
         <v>11</v>
       </c>
+      <c r="F19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D34">
-    <sortCondition ref="A2:A34"/>
+  <sortState ref="B2:E34">
+    <sortCondition ref="B2:B34"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3:F19" r:id="rId2" display="joe@acme.com"/>
+    <hyperlink ref="G2" r:id="rId3"/>
+    <hyperlink ref="G3:G19" r:id="rId4" display="www.smithpiano.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>